<commit_message>
hub node bigger. Only displaying prefixes in leaf nodes
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -63,9 +63,6 @@
     <t>untergehen</t>
   </si>
   <si>
-    <t>zugeen</t>
-  </si>
-  <si>
     <t>gehen</t>
   </si>
   <si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t>#Verb</t>
+  </si>
+  <si>
+    <t>zugehen</t>
   </si>
 </sst>
 </file>
@@ -550,7 +550,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -562,7 +564,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -579,13 +581,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -593,16 +595,16 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -610,13 +612,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -624,13 +626,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -638,13 +640,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -652,13 +654,13 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -666,13 +668,13 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -680,13 +682,13 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -694,16 +696,16 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
         <v>38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -711,13 +713,13 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -725,98 +727,98 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
         <v>42</v>
-      </c>
-      <c r="E12" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
         <v>44</v>
-      </c>
-      <c r="E13" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
         <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" t="s">
         <v>24</v>
-      </c>
-      <c r="E15" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
         <v>26</v>
-      </c>
-      <c r="E16" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
         <v>21</v>
       </c>
-      <c r="B17" t="s">
-        <v>22</v>
-      </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Displays translation when clicked, then shrinks back to normal. Nearly MVP
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t>Root</t>
   </si>
@@ -87,33 +87,12 @@
     <t>stellen</t>
   </si>
   <si>
-    <t>to turn off</t>
-  </si>
-  <si>
-    <t>to lean on</t>
-  </si>
-  <si>
-    <t>to attempt</t>
-  </si>
-  <si>
-    <t>to arrange</t>
-  </si>
-  <si>
-    <t>to establish</t>
-  </si>
-  <si>
     <t>to order</t>
   </si>
   <si>
     <t>to exit</t>
   </si>
   <si>
-    <t>to concern something</t>
-  </si>
-  <si>
-    <t>to tackle</t>
-  </si>
-  <si>
     <t>to go out</t>
   </si>
   <si>
@@ -135,31 +114,31 @@
     <t>to skip</t>
   </si>
   <si>
-    <t>to ignore</t>
-  </si>
-  <si>
-    <t>to put down</t>
-  </si>
-  <si>
     <t>to bypass</t>
   </si>
   <si>
     <t>to sink</t>
   </si>
   <si>
-    <t>to descend</t>
-  </si>
-  <si>
-    <t>to approach</t>
-  </si>
-  <si>
-    <t>to close</t>
-  </si>
-  <si>
     <t>#Verb</t>
   </si>
   <si>
     <t>zugehen</t>
+  </si>
+  <si>
+    <t>to approach / to close</t>
+  </si>
+  <si>
+    <t>to tackle / to concern something</t>
+  </si>
+  <si>
+    <t>to put down / to turn off</t>
+  </si>
+  <si>
+    <t>to lean on / to attempt</t>
+  </si>
+  <si>
+    <t>to arrange / to establish</t>
   </si>
 </sst>
 </file>
@@ -548,23 +527,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -576,7 +555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -587,10 +566,10 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -601,13 +580,10 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -618,10 +594,10 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -632,10 +608,10 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -646,10 +622,10 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -660,10 +636,10 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -674,10 +650,10 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -688,10 +664,10 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -702,13 +678,10 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -719,10 +692,10 @@
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -733,15 +706,12 @@
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -750,13 +720,10 @@
         <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -767,13 +734,10 @@
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -784,13 +748,10 @@
         <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -801,10 +762,7 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -818,7 +776,7 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
untergehen is separable, fixed this error. Also, made the fill of the text stay the same when the nodes inflate when clicked
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -530,7 +530,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -703,7 +703,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
         <v>32</v>

</xml_diff>